<commit_message>
tax report full functionality
</commit_message>
<xml_diff>
--- a/report_creation_program/report_creation_program/bin/Debug/InventoryReport.xlsx
+++ b/report_creation_program/report_creation_program/bin/Debug/InventoryReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College Homework\CAPSTONE\TEST REPO\report_creation_program\report_creation_program\report_creation_program\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/016be9303c01b4f8/Documents/SCHOOL STUFF/05 Summer 2021/Capstone/malloyethan11/report_creation_program/report_creation_program/report_creation_program/bin/Debug/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8AEAE08-9B37-4E7E-9BE3-BEAE150310FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{22488861-E4B1-4E7E-8D3E-BFB1FF0FC5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15450" yWindow="1095" windowWidth="13350" windowHeight="11835" xr2:uid="{34E8B858-753D-43B5-965A-19E4759962F2}"/>
+    <workbookView xWindow="-26835" yWindow="660" windowWidth="22980" windowHeight="13770" xr2:uid="{8B7631AE-5FF9-47B8-8A5E-99114D21431E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A333E22-65A3-4C08-9EA1-250FA2273211}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6262397-9902-4170-9AD8-8752DF0A6E58}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
inventory report full functionality
</commit_message>
<xml_diff>
--- a/report_creation_program/report_creation_program/bin/Debug/InventoryReport.xlsx
+++ b/report_creation_program/report_creation_program/bin/Debug/InventoryReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/016be9303c01b4f8/Documents/SCHOOL STUFF/05 Summer 2021/Capstone/malloyethan11/report_creation_program/report_creation_program/report_creation_program/bin/Debug/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallo\OneDrive\Documents\SCHOOL STUFF\05 Summer 2021\Capstone\malloyethan11\report_creation_program\report_creation_program\report_creation_program\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22488861-E4B1-4E7E-8D3E-BFB1FF0FC5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FF5B21B-2A43-4336-83C1-49EB4EEF9104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26835" yWindow="660" windowWidth="22980" windowHeight="13770" xr2:uid="{8B7631AE-5FF9-47B8-8A5E-99114D21431E}"/>
+    <workbookView xWindow="-26490" yWindow="1005" windowWidth="22980" windowHeight="13770" xr2:uid="{A6371654-A946-44A5-BFE8-226E2CE8CBDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>SKU</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t>840029425619​</t>
+  </si>
+  <si>
+    <t>TEST01</t>
+  </si>
+  <si>
+    <t>Test Item</t>
+  </si>
+  <si>
+    <t>TestVendor</t>
+  </si>
+  <si>
+    <t>123456789101​</t>
   </si>
 </sst>
 </file>
@@ -474,8 +486,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6262397-9902-4170-9AD8-8752DF0A6E58}">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2793097E-7EB9-48CE-8AEF-31AFA40A032A}">
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -524,7 +536,7 @@
         <v>16.5</v>
       </c>
       <c r="F2">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -576,7 +588,7 @@
         <v>24.95</v>
       </c>
       <c r="F4">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -602,7 +614,7 @@
         <v>49.95</v>
       </c>
       <c r="F5">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -635,6 +647,32 @@
       </c>
       <c r="H6" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7">
+        <v>11.1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New report generation method.
</commit_message>
<xml_diff>
--- a/report_creation_program/report_creation_program/bin/Debug/InventoryReport.xlsx
+++ b/report_creation_program/report_creation_program/bin/Debug/InventoryReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallo\OneDrive\Documents\SCHOOL STUFF\05 Summer 2021\Capstone\malloyethan11\report_creation_program\report_creation_program\report_creation_program\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College Homework\CAPSTONE\report_creation_program\report_creation_program\report_creation_program\report_creation_program\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FF5B21B-2A43-4336-83C1-49EB4EEF9104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{90CE0B7E-65CE-4680-9529-347DEE834690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26490" yWindow="1005" windowWidth="22980" windowHeight="13770" xr2:uid="{A6371654-A946-44A5-BFE8-226E2CE8CBDC}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{14C25800-1D73-43F5-921A-A6B20EA56B4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -486,7 +486,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2793097E-7EB9-48CE-8AEF-31AFA40A032A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1383B337-0A0D-4088-AC9F-A88F1CD7E5DE}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>